<commit_message>
docs: aggiornamento documentazione feature dashboard e layout
</commit_message>
<xml_diff>
--- a/0. Requirements/PortfolioDataMin1.xlsx
+++ b/0. Requirements/PortfolioDataMin1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PerixMonitor\0. Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF35C4-3679-4A23-9E01-49AFAEF42F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7679AD-03CA-4134-AA59-AE568DB3E003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
   </bookViews>
@@ -207,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -221,7 +221,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -564,7 +563,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -616,16 +615,16 @@
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>255.42699999999999</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>242.5</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="9">
         <v>45355</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -645,25 +644,25 @@
       <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>786.29</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>28.88</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>45355</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>28.88</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="8">
         <v>28.88</v>
       </c>
     </row>

</xml_diff>